<commit_message>
correzione formula nastro trasportatore
</commit_message>
<xml_diff>
--- a/FogliCalcolo/NastroTrasportatore/Nastro.xlsx
+++ b/FogliCalcolo/NastroTrasportatore/Nastro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\NastroTrasportatore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\NastroTrasportatore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1371FB81-5F77-4959-A288-9E645BE347E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB152389-F559-4B85-982A-2BEB4C81A60F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-60" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{38F28402-0782-459F-A055-4B2B36D37780}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38F28402-0782-459F-A055-4B2B36D37780}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle" sheetId="2" r:id="rId1"/>
@@ -751,34 +751,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -793,6 +772,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -877,7 +877,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1002,7 +1002,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3185.6637272727276</c:v>
+                  <c:v>6371.3274545454551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1088,7 +1088,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.0529277386363645</c:v>
+                  <c:v>6.1058554772727289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1191,7 +1191,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="816908111"/>
@@ -1278,7 +1278,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1310,7 +1310,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="816910191"/>
@@ -1352,7 +1352,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1382,7 +1382,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2280,13 +2280,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -2299,7 +2299,7 @@
       <c r="B4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="38" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="3">
@@ -2334,14 +2334,14 @@
     </row>
     <row r="7" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
@@ -2511,26 +2511,26 @@
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51" t="s">
+      <c r="D19" s="44"/>
+      <c r="E19" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="52"/>
+      <c r="F19" s="45"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
@@ -2700,7 +2700,7 @@
   <dimension ref="B1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,7 +2807,7 @@
         <v>77</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" t="s">
@@ -2832,11 +2832,11 @@
       </c>
       <c r="C14" s="3">
         <f>IF($C$12=1,1/110*(B14/1000+4)*(B14/1000)^2,1/55*(B14/1000+4)*(B14/1000)^2)</f>
-        <v>1.5054545454545451E-2</v>
+        <v>3.0109090909090901E-2</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" ref="D14:D19" si="0">$C$11/C14</f>
-        <v>9.8407586330291661</v>
+        <v>4.920379316514583</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -2846,11 +2846,11 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ref="C15:C19" si="1">IF($C$12=1,1/110*(B15/1000+4)*(B15/1000)^2,1/55*(B15/1000+4)*(B15/1000)^2)</f>
-        <v>2.0936363636363631E-2</v>
+        <v>4.1872727272727263E-2</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="0"/>
-        <v>7.0761164986089007</v>
+        <v>3.5380582493044503</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -2859,11 +2859,11 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" si="1"/>
-        <v>2.7927272727272731E-2</v>
+        <v>5.5854545454545462E-2</v>
       </c>
       <c r="D16" s="31">
         <f t="shared" si="0"/>
-        <v>5.3047839506172831</v>
+        <v>2.6523919753086416</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2872,11 +2872,11 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" si="1"/>
-        <v>3.6081818181818187E-2</v>
+        <v>7.2163636363636374E-2</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
-        <v>4.1058947584520764</v>
+        <v>2.0529473792260382</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2885,11 +2885,11 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
-        <v>4.5454545454545456E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>3.2592592592592591</v>
+        <v>1.6296296296296295</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2898,11 +2898,11 @@
       </c>
       <c r="C19" s="34">
         <f t="shared" si="1"/>
-        <v>3.6081818181818187E-2</v>
+        <v>7.2163636363636374E-2</v>
       </c>
       <c r="D19" s="35">
         <f t="shared" si="0"/>
-        <v>4.1058947584520764</v>
+        <v>2.0529473792260382</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="C28" s="3">
         <f>C23*C19*C6*(C4+C24)*9.81*C10</f>
-        <v>3185.6637272727276</v>
+        <v>6371.3274545454551</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>8</v>
@@ -2998,7 +2998,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="3">
-        <f>C16*C6*C5*9.81</f>
+        <f>C19*C6*C5*9.81</f>
         <v>0</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="C30" s="3">
         <f>0.0115*C6*C19*9.81</f>
-        <v>3.0529277386363645</v>
+        <v>6.1058554772727289</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>8</v>
@@ -3033,7 +3033,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="6">
         <f>SUM(C25,C28,C29,C30,C31)</f>
-        <v>10399.066655011362</v>
+        <v>13587.783310022727</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>8</v>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="C37" s="17">
         <f>C32/(EXP(C35*RADIANS(C36))-1)</f>
-        <v>6639.1186741876254</v>
+        <v>8674.9040954472348</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
@@ -3089,9 +3089,9 @@
       <c r="B38" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="17">
         <f>C37+C32</f>
-        <v>17038.185329198986</v>
+        <v>22262.687405469962</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="C40" s="17">
         <f>2*(C26+C37)/9.81</f>
-        <v>2233.5410141055299</v>
+        <v>2648.5839134448997</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>52</v>
@@ -3150,8 +3150,8 @@
         <v>29</v>
       </c>
       <c r="C44" s="3">
-        <f>_xlfn.CEILING.MATH(C38/(5*B19))</f>
-        <v>4</v>
+        <f>_xlfn.CEILING.MATH(C38/(C43*B19))</f>
+        <v>5</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="C45" s="3">
         <f>50*C44*B16/1000*9.81</f>
-        <v>1569.6000000000001</v>
+        <v>1962</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -3190,12 +3190,12 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="45"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="48"/>
     </row>
     <row r="50" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B50" s="20" t="s">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="C52" s="17">
         <f>0.001*C32*D19/(C50*C51)</f>
-        <v>59.302046210562381</v>
+        <v>38.743061299725632</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>64</v>
@@ -3249,12 +3249,12 @@
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="49" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="17">
         <f>2*D19/C54</f>
-        <v>18.248421148675895</v>
+        <v>9.1242105743379476</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>18</v>
@@ -3262,10 +3262,10 @@
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="46"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="17">
         <f>60*C55/(2*PI())</f>
-        <v>174.25958576606709</v>
+        <v>87.129792883033545</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>19</v>
@@ -3273,12 +3273,12 @@
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="42"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="52"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
@@ -3362,11 +3362,11 @@
       <c r="B64" s="2"/>
       <c r="C64" s="17">
         <f>C61/C56</f>
-        <v>17.043538735292557</v>
+        <v>34.087077470585115</v>
       </c>
       <c r="D64" s="17">
         <f>D61/C56</f>
-        <v>8.4930765414925879</v>
+        <v>16.986153082985176</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>73</v>
@@ -3384,11 +3384,11 @@
       </c>
       <c r="C66" s="25">
         <f>3^0.5/3*$C$52*1000/($C$58*C63)</f>
-        <v>93.038185715119056</v>
+        <v>60.783469757137944</v>
       </c>
       <c r="D66" s="25">
         <f>3^0.5/3*$C$52*1000/($C$58*D63)</f>
-        <v>92.037775116031753</v>
+        <v>60.129884060824637</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>21</v>

</xml_diff>